<commit_message>
convert Inf to char
</commit_message>
<xml_diff>
--- a/tables/results/TableS4-survival-results-table.xlsx
+++ b/tables/results/TableS4-survival-results-table.xlsx
@@ -17,14 +17,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t xml:space="preserve">term</t>
   </si>
   <si>
-    <t xml:space="preserve">estimate</t>
-  </si>
-  <si>
     <t xml:space="preserve">std.error</t>
   </si>
   <si>
@@ -118,37 +115,85 @@
     <t xml:space="preserve">hgg_groupHGG</t>
   </si>
   <si>
+    <t xml:space="preserve">1572945838334.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2068.45013556778</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.32242977898441</t>
+  </si>
+  <si>
     <t xml:space="preserve">B_cell</t>
   </si>
   <si>
+    <t xml:space="preserve">8.60269538760554e+68</t>
+  </si>
+  <si>
     <t xml:space="preserve">Macrophage_M1</t>
   </si>
   <si>
     <t xml:space="preserve">Macrophage_M2</t>
   </si>
   <si>
+    <t xml:space="preserve">1.35246231730248e+169</t>
+  </si>
+  <si>
     <t xml:space="preserve">Monocyte</t>
   </si>
   <si>
+    <t xml:space="preserve">2.3484686232254e+30</t>
+  </si>
+  <si>
     <t xml:space="preserve">Myeloid_dendritic_cell</t>
   </si>
   <si>
+    <t xml:space="preserve">1.06479257434283e+28</t>
+  </si>
+  <si>
     <t xml:space="preserve">Neutrophil</t>
   </si>
   <si>
+    <t xml:space="preserve">1.50489322180708e+108</t>
+  </si>
+  <si>
     <t xml:space="preserve">NK_cell</t>
   </si>
   <si>
+    <t xml:space="preserve">2823706437591606272</t>
+  </si>
+  <si>
     <t xml:space="preserve">T_cell_CD4_non_regulatory</t>
   </si>
   <si>
+    <t xml:space="preserve">3.94583133618291e+46</t>
+  </si>
+  <si>
     <t xml:space="preserve">T_cell_CD8</t>
   </si>
   <si>
+    <t xml:space="preserve">1.26769440002487e+103</t>
+  </si>
+  <si>
     <t xml:space="preserve">T_cell_regulatory_Tregs</t>
   </si>
   <si>
+    <t xml:space="preserve">4.88417817394597e+131</t>
+  </si>
+  <si>
     <t xml:space="preserve">CD274</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.18045003090112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.60975614839146</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29.0506378211092</t>
   </si>
 </sst>
 </file>
@@ -502,111 +547,96 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>0.604322792977182</v>
+        <v>0.47844633411542</v>
       </c>
       <c r="C2" t="n">
-        <v>0.47844633411542</v>
+        <v>1.26309420699082</v>
       </c>
       <c r="D2" t="n">
-        <v>1.26309420699082</v>
+        <v>0.206555325652364</v>
       </c>
       <c r="E2" t="n">
-        <v>0.206555325652364</v>
+        <v>0.716472946394793</v>
       </c>
       <c r="F2" t="n">
-        <v>0.716472946394793</v>
+        <v>4.67421099034643</v>
       </c>
       <c r="G2" t="n">
-        <v>4.67421099034643</v>
-      </c>
-      <c r="H2" t="n">
         <v>1.83001249184929</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" t="n">
-        <v>1.14993901726137</v>
+        <v>0.372657336884355</v>
       </c>
       <c r="C3" t="n">
-        <v>0.372657336884355</v>
+        <v>3.08578123504979</v>
       </c>
       <c r="D3" t="n">
-        <v>3.08578123504979</v>
+        <v>0.00203018130922217</v>
       </c>
       <c r="E3" t="n">
-        <v>0.00203018130922217</v>
+        <v>1.52126778819255</v>
       </c>
       <c r="F3" t="n">
-        <v>1.52126778819255</v>
+        <v>6.55569394190831</v>
       </c>
       <c r="G3" t="n">
-        <v>6.55569394190831</v>
-      </c>
-      <c r="H3" t="n">
         <v>3.15800032030938</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.739269902039682</v>
+        <v>0.475306896240576</v>
       </c>
       <c r="C4" t="n">
-        <v>0.475306896240576</v>
+        <v>-1.55535277919785</v>
       </c>
       <c r="D4" t="n">
-        <v>-1.55535277919785</v>
+        <v>0.119862073744265</v>
       </c>
       <c r="E4" t="n">
-        <v>0.119862073744265</v>
+        <v>0.188086314793378</v>
       </c>
       <c r="F4" t="n">
-        <v>0.188086314793378</v>
+        <v>1.21205164266067</v>
       </c>
       <c r="G4" t="n">
-        <v>1.21205164266067</v>
-      </c>
-      <c r="H4" t="n">
         <v>0.477462382609672</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" t="n">
-        <v>0.324903264866795</v>
+        <v>0.461653149975373</v>
       </c>
       <c r="C5" t="n">
-        <v>0.461653149975373</v>
+        <v>0.703782189906269</v>
       </c>
       <c r="D5" t="n">
-        <v>0.703782189906269</v>
+        <v>0.481568426704985</v>
       </c>
       <c r="E5" t="n">
-        <v>0.481568426704985</v>
+        <v>0.55994300207926</v>
       </c>
       <c r="F5" t="n">
-        <v>0.55994300207926</v>
+        <v>3.42029502566414</v>
       </c>
       <c r="G5" t="n">
-        <v>3.42029502566414</v>
-      </c>
-      <c r="H5" t="n">
         <v>1.38389676806731</v>
       </c>
     </row>
@@ -626,39 +656,39 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>19</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>20</v>
-      </c>
-      <c r="J1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" t="n">
         <v>13</v>
@@ -690,7 +720,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" t="n">
         <v>7</v>
@@ -722,7 +752,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" t="n">
         <v>26</v>
@@ -754,7 +784,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" t="n">
         <v>12</v>
@@ -786,7 +816,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" t="n">
         <v>8</v>
@@ -852,163 +882,142 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" t="n">
-        <v>0.665161143509664</v>
+        <v>0.454121173826659</v>
       </c>
       <c r="C2" t="n">
-        <v>0.454121173826659</v>
+        <v>1.4647217127197</v>
       </c>
       <c r="D2" t="n">
-        <v>1.4647217127197</v>
+        <v>0.142996858543784</v>
       </c>
       <c r="E2" t="n">
-        <v>0.142996858543784</v>
+        <v>0.798596072930393</v>
       </c>
       <c r="F2" t="n">
-        <v>0.798596072930393</v>
+        <v>4.73613919898317</v>
       </c>
       <c r="G2" t="n">
-        <v>4.73613919898317</v>
-      </c>
-      <c r="H2" t="n">
         <v>1.94480388861182</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" t="n">
-        <v>3.16205585245876</v>
+        <v>0.614572617817878</v>
       </c>
       <c r="C3" t="n">
-        <v>0.614572617817878</v>
+        <v>5.14512973859145</v>
       </c>
       <c r="D3" t="n">
-        <v>5.14512973859145</v>
+        <v>0.000000267335988648007</v>
       </c>
       <c r="E3" t="n">
-        <v>0.000000267335988648007</v>
+        <v>7.08171178235642</v>
       </c>
       <c r="F3" t="n">
-        <v>7.08171178235642</v>
+        <v>78.7750284868543</v>
       </c>
       <c r="G3" t="n">
-        <v>78.7750284868543</v>
-      </c>
-      <c r="H3" t="n">
         <v>23.6191034417232</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" t="n">
-        <v>-1.01079984269197</v>
+        <v>0.312839353936692</v>
       </c>
       <c r="C4" t="n">
-        <v>0.312839353936692</v>
+        <v>-3.23105079323403</v>
       </c>
       <c r="D4" t="n">
-        <v>-3.23105079323403</v>
+        <v>0.00123336020308562</v>
       </c>
       <c r="E4" t="n">
-        <v>0.00123336020308562</v>
+        <v>0.197117809867498</v>
       </c>
       <c r="F4" t="n">
-        <v>0.197117809867498</v>
+        <v>0.671899854215695</v>
       </c>
       <c r="G4" t="n">
-        <v>0.671899854215695</v>
-      </c>
-      <c r="H4" t="n">
         <v>0.363927778155624</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.257676506453152</v>
+        <v>0.299884699761876</v>
       </c>
       <c r="C5" t="n">
-        <v>0.299884699761876</v>
+        <v>-0.85925192801687</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.85925192801687</v>
+        <v>0.390201539716764</v>
       </c>
       <c r="E5" t="n">
-        <v>0.390201539716764</v>
+        <v>0.429368515844325</v>
       </c>
       <c r="F5" t="n">
-        <v>0.429368515844325</v>
+        <v>1.39108873702023</v>
       </c>
       <c r="G5" t="n">
-        <v>1.39108873702023</v>
-      </c>
-      <c r="H5" t="n">
         <v>0.772845202108501</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" t="n">
-        <v>-2.69329325555705</v>
+        <v>1.02177506179121</v>
       </c>
       <c r="C6" t="n">
-        <v>1.02177506179121</v>
+        <v>-2.63589644753672</v>
       </c>
       <c r="D6" t="n">
-        <v>-2.63589644753672</v>
+        <v>0.00839153358374639</v>
       </c>
       <c r="E6" t="n">
-        <v>0.00839153358374639</v>
+        <v>0.00913231938217678</v>
       </c>
       <c r="F6" t="n">
-        <v>0.00913231938217678</v>
+        <v>0.501249682315998</v>
       </c>
       <c r="G6" t="n">
-        <v>0.501249682315998</v>
-      </c>
-      <c r="H6" t="n">
         <v>0.0676577577896604</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" t="n">
-        <v>1.73202004740856</v>
+        <v>0.237798791317952</v>
       </c>
       <c r="C7" t="n">
-        <v>0.237798791317952</v>
+        <v>7.28355277926011</v>
       </c>
       <c r="D7" t="n">
-        <v>7.28355277926011</v>
+        <v>0.000000000000325141633705587</v>
       </c>
       <c r="E7" t="n">
-        <v>0.000000000000325141633705587</v>
+        <v>3.54643538051519</v>
       </c>
       <c r="F7" t="n">
-        <v>3.54643538051519</v>
+        <v>9.00785625654152</v>
       </c>
       <c r="G7" t="n">
-        <v>9.00785625654152</v>
-      </c>
-      <c r="H7" t="n">
         <v>5.65205981309416</v>
       </c>
     </row>
@@ -1048,97 +1057,85 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" t="n">
-        <v>7.38518165105578</v>
+        <v>2.64087618039762</v>
       </c>
       <c r="C2" t="n">
-        <v>2.64087618039762</v>
+        <v>2.79648917502214</v>
       </c>
       <c r="D2" t="n">
-        <v>2.79648917502214</v>
+        <v>0.0051661141554533</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0051661141554533</v>
+        <v>9.10805739556573</v>
       </c>
       <c r="F2" t="n">
-        <v>9.10805739556573</v>
+        <v>285273.558212938</v>
       </c>
       <c r="G2" t="n">
-        <v>285273.558212938</v>
-      </c>
-      <c r="H2" t="n">
         <v>1611.92057547532</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" t="n">
-        <v>22.181455478365</v>
+        <v>7.32532067488232</v>
       </c>
       <c r="C3" t="n">
-        <v>7.32532067488232</v>
+        <v>3.02805248573249</v>
       </c>
       <c r="D3" t="n">
-        <v>3.02805248573249</v>
+        <v>0.00246135333921797</v>
       </c>
       <c r="E3" t="n">
-        <v>0.00246135333921797</v>
+        <v>2500.11192633725</v>
       </c>
       <c r="F3" t="n">
-        <v>2500.11192633725</v>
+        <v>7389379609457043</v>
       </c>
       <c r="G3" t="n">
-        <v>7389379609457043</v>
-      </c>
-      <c r="H3" t="n">
         <v>4298171249.47772</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" t="n">
-        <v>-28.872470714387</v>
+        <v>1.37753051015512</v>
       </c>
       <c r="C4" t="n">
-        <v>1.37753051015512</v>
+        <v>-20.959587102819</v>
       </c>
       <c r="D4" t="n">
-        <v>-20.959587102819</v>
+        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000153412046828091</v>
       </c>
       <c r="E4" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000153412046828091</v>
+        <v>0.0000000000000194217873077806</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0000000000000194217873077806</v>
+        <v>0.00000000000429933598658414</v>
       </c>
       <c r="G4" t="n">
-        <v>0.00000000000429933598658414</v>
-      </c>
-      <c r="H4" t="n">
         <v>0.000000000000288965030922644</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" t="e">
+        <v>29</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="e">
         <v>#N/A</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0</v>
       </c>
       <c r="D5" t="e">
         <v>#N/A</v>
@@ -1150,9 +1147,6 @@
         <v>#N/A</v>
       </c>
       <c r="G5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H5" t="e">
         <v>#N/A</v>
       </c>
     </row>
@@ -1192,111 +1186,96 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" t="n">
-        <v>14.3842210389594</v>
+        <v>6.98979694342947</v>
       </c>
       <c r="C2" t="n">
-        <v>6.98979694342947</v>
+        <v>2.05788825560674</v>
       </c>
       <c r="D2" t="n">
-        <v>2.05788825560674</v>
+        <v>0.0396008613847964</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0396008613847964</v>
-      </c>
-      <c r="F2" t="n">
         <v>1.98272224290025</v>
       </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
       <c r="G2" t="n">
-        <v>1572945838334.15</v>
-      </c>
-      <c r="H2" t="n">
         <v>1765988.30702315</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.211206267593403</v>
+        <v>4.00301291683135</v>
       </c>
       <c r="C3" t="n">
-        <v>4.00301291683135</v>
+        <v>-0.0527618251505884</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.0527618251505884</v>
+        <v>0.957921678227888</v>
       </c>
       <c r="E3" t="n">
-        <v>0.957921678227888</v>
-      </c>
-      <c r="F3" t="n">
         <v>0.000316886334627329</v>
       </c>
+      <c r="F3" t="s">
+        <v>33</v>
+      </c>
       <c r="G3" t="n">
-        <v>2068.45013556778</v>
-      </c>
-      <c r="H3" t="n">
         <v>0.80960705395857</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" t="n">
-        <v>22.5492903011863</v>
+        <v>15663.1915129564</v>
       </c>
       <c r="C4" t="n">
-        <v>15663.1915129564</v>
+        <v>0.00143963573978737</v>
       </c>
       <c r="D4" t="n">
-        <v>0.00143963573978737</v>
+        <v>0.998851337266821</v>
       </c>
       <c r="E4" t="n">
-        <v>0.998851337266821</v>
-      </c>
-      <c r="F4" t="n">
         <v>0</v>
       </c>
-      <c r="G4" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="H4" t="n">
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" t="n">
         <v>6209152816.90122</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" t="n">
-        <v>0.103823720175267</v>
+        <v>0.693887226261366</v>
       </c>
       <c r="C5" t="n">
-        <v>0.693887226261366</v>
+        <v>0.149626216258029</v>
       </c>
       <c r="D5" t="n">
-        <v>0.149626216258029</v>
+        <v>0.881059523440836</v>
       </c>
       <c r="E5" t="n">
-        <v>0.881059523440836</v>
-      </c>
-      <c r="F5" t="n">
         <v>0.2847424325918</v>
       </c>
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
       <c r="G5" t="n">
-        <v>4.32242977898441</v>
-      </c>
-      <c r="H5" t="n">
         <v>1.10940487198104</v>
       </c>
     </row>
@@ -1336,345 +1315,303 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B2" t="n">
-        <v>29.4777283445468</v>
+        <v>65.9451574467056</v>
       </c>
       <c r="C2" t="n">
-        <v>65.9451574467056</v>
+        <v>0.447003684362564</v>
       </c>
       <c r="D2" t="n">
-        <v>0.447003684362564</v>
+        <v>0.654872399695274</v>
       </c>
       <c r="E2" t="n">
-        <v>0.654872399695274</v>
-      </c>
-      <c r="F2" t="n">
         <v>0.0000000000000000000000000000000000000000000467083980799242</v>
       </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
       <c r="G2" t="n">
-        <v>860269538760554131238491782831514333871429064586502058669576990752768</v>
-      </c>
-      <c r="H2" t="n">
         <v>6338912530746.95</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="n">
+        <v>24841596.4241147</v>
+      </c>
+      <c r="C3" t="n">
+        <v>-0.00360331808662127</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.997124974352533</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
         <v>34</v>
       </c>
-      <c r="B3" t="n">
-        <v>-89512.1736955588</v>
-      </c>
-      <c r="C3" t="n">
-        <v>24841596.4241147</v>
-      </c>
-      <c r="D3" t="n">
-        <v>-0.00360331808662127</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.997124974352533</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="H3" t="n">
+      <c r="G3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B4" t="n">
-        <v>79.8185644322824</v>
+        <v>157.972414593224</v>
       </c>
       <c r="C4" t="n">
-        <v>157.972414593224</v>
+        <v>0.505269003058629</v>
       </c>
       <c r="D4" t="n">
-        <v>0.505269003058629</v>
+        <v>0.613369910816791</v>
       </c>
       <c r="E4" t="n">
-        <v>0.613369910816791</v>
-      </c>
-      <c r="F4" t="n">
         <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000157906133407611</v>
       </c>
+      <c r="F4" t="s">
+        <v>40</v>
+      </c>
       <c r="G4" t="n">
-        <v>13524623173024820504180205035559133824102320133751743255623490805291124796883935870661673627956844236528112961223452050875195365487964197580387951877347310002500106452992</v>
-      </c>
-      <c r="H4" t="n">
         <v>46212779088120034539933417387065344</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B5" t="n">
-        <v>40.7997722959806</v>
+        <v>14.8633057493278</v>
       </c>
       <c r="C5" t="n">
-        <v>14.8633057493278</v>
+        <v>2.74499986638744</v>
       </c>
       <c r="D5" t="n">
-        <v>2.74499986638744</v>
+        <v>0.0060510922336591</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0060510922336591</v>
-      </c>
-      <c r="F5" t="n">
         <v>116801.166454098</v>
       </c>
+      <c r="F5" t="s">
+        <v>42</v>
+      </c>
       <c r="G5" t="n">
-        <v>2348468623225396798932681490432</v>
-      </c>
-      <c r="H5" t="n">
         <v>523740273965613504</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B6" t="n">
-        <v>18.325707058351</v>
+        <v>23.5766860637712</v>
       </c>
       <c r="C6" t="n">
-        <v>23.5766860637712</v>
+        <v>0.777280870126654</v>
       </c>
       <c r="D6" t="n">
-        <v>0.777280870126654</v>
+        <v>0.436993078868274</v>
       </c>
       <c r="E6" t="n">
-        <v>0.436993078868274</v>
-      </c>
-      <c r="F6" t="n">
         <v>0.00000000000077667958706768</v>
       </c>
+      <c r="F6" t="s">
+        <v>44</v>
+      </c>
       <c r="G6" t="n">
-        <v>10647925743428290208017154048</v>
-      </c>
-      <c r="H6" t="n">
         <v>90939686.4385031</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B7" t="n">
-        <v>20.5549906641994</v>
+        <v>116.600571810765</v>
       </c>
       <c r="C7" t="n">
-        <v>116.600571810765</v>
+        <v>0.176285504822041</v>
       </c>
       <c r="D7" t="n">
-        <v>0.176285504822041</v>
+        <v>0.860069649178577</v>
       </c>
       <c r="E7" t="n">
-        <v>0.860069649178577</v>
-      </c>
-      <c r="F7" t="n">
         <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000474605051084553</v>
       </c>
+      <c r="F7" t="s">
+        <v>46</v>
+      </c>
       <c r="G7" t="n">
-        <v>1504893221807084361204800523442514737869349796556619306931407136429299827155534790747041980208208307814400000</v>
-      </c>
-      <c r="H7" t="n">
         <v>845121248.349933</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B8" t="n">
-        <v>-17.9048786820116</v>
+        <v>30.8115155144595</v>
       </c>
       <c r="C8" t="n">
-        <v>30.8115155144595</v>
+        <v>-0.58110996434463</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.58110996434463</v>
+        <v>0.5611663434077</v>
       </c>
       <c r="E8" t="n">
-        <v>0.5611663434077</v>
-      </c>
-      <c r="F8" t="n">
         <v>0.0000000000000000000000000000000000993574494765512</v>
       </c>
+      <c r="F8" t="s">
+        <v>48</v>
+      </c>
       <c r="G8" t="n">
-        <v>2823706437591606272</v>
-      </c>
-      <c r="H8" t="n">
         <v>0.0000000167498140201503</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B9" t="n">
-        <v>39.5816073792588</v>
+        <v>34.5465361079373</v>
       </c>
       <c r="C9" t="n">
-        <v>34.5465361079373</v>
+        <v>1.14574749999797</v>
       </c>
       <c r="D9" t="n">
-        <v>1.14574749999797</v>
+        <v>0.25189964364869</v>
       </c>
       <c r="E9" t="n">
-        <v>0.25189964364869</v>
-      </c>
-      <c r="F9" t="n">
         <v>0.000000000000608147354514014</v>
       </c>
+      <c r="F9" t="s">
+        <v>50</v>
+      </c>
       <c r="G9" t="n">
-        <v>39458313361829077998738475474416547601508728832</v>
-      </c>
-      <c r="H9" t="n">
         <v>154907936803062144</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="B10" t="n">
-        <v>-85.7067715212463</v>
+        <v>164.855190435033</v>
       </c>
       <c r="C10" t="n">
-        <v>164.855190435033</v>
+        <v>-0.5198912530147</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.5198912530147</v>
+        <v>0.603139372257192</v>
       </c>
       <c r="E10" t="n">
-        <v>0.603139372257192</v>
-      </c>
-      <c r="F10" t="n">
         <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000283811220481693</v>
       </c>
+      <c r="F10" t="s">
+        <v>52</v>
+      </c>
       <c r="G10" t="n">
-        <v>12676944000248749507337565624545422676732924476288491241726104614852551773963786590299333539421203988480</v>
-      </c>
-      <c r="H10" t="n">
         <v>0.0000000000000000000000000000000000000599821552521129</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="B11" t="n">
-        <v>-104.200133651008</v>
+        <v>207.873606394647</v>
       </c>
       <c r="C11" t="n">
-        <v>207.873606394647</v>
+        <v>-0.50126678157103</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.50126678157103</v>
+        <v>0.616183380381179</v>
       </c>
       <c r="E11" t="n">
-        <v>0.616183380381179</v>
-      </c>
-      <c r="F11" t="n">
         <v>6.36974996404952e-223</v>
       </c>
+      <c r="F11" t="s">
+        <v>54</v>
+      </c>
       <c r="G11" t="n">
-        <v>488417817394596697097673161802831033771860423571919259029488622014314034732718283277141427314138519889771858339435657345750500638720</v>
-      </c>
-      <c r="H11" t="n">
         <v>0.000000000000000000000000000000000000000000000557772298952752</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B12" t="n">
-        <v>-7.20841135589492</v>
+        <v>2.80418927214936</v>
       </c>
       <c r="C12" t="n">
-        <v>2.80418927214936</v>
+        <v>-2.57058659609299</v>
       </c>
       <c r="D12" t="n">
-        <v>-2.57058659609299</v>
+        <v>0.0101526440656152</v>
       </c>
       <c r="E12" t="n">
-        <v>0.0101526440656152</v>
-      </c>
-      <c r="F12" t="n">
         <v>0.00000303736153615593</v>
       </c>
+      <c r="F12" t="s">
+        <v>56</v>
+      </c>
       <c r="G12" t="n">
-        <v>0.18045003090112</v>
-      </c>
-      <c r="H12" t="n">
         <v>0.000740332346353454</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.25793992615902</v>
+        <v>1.0951663933398</v>
       </c>
       <c r="C13" t="n">
-        <v>1.0951663933398</v>
+        <v>-0.235525786517619</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.235525786517619</v>
+        <v>0.813800666948844</v>
       </c>
       <c r="E13" t="n">
-        <v>0.813800666948844</v>
-      </c>
-      <c r="F13" t="n">
         <v>0.0903172674058606</v>
       </c>
+      <c r="F13" t="s">
+        <v>57</v>
+      </c>
       <c r="G13" t="n">
-        <v>6.60975614839146</v>
-      </c>
-      <c r="H13" t="n">
         <v>0.772641646264168</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" t="n">
-        <v>1.26052610437748</v>
+        <v>1.07579238765984</v>
       </c>
       <c r="C14" t="n">
-        <v>1.07579238765984</v>
+        <v>1.17171874316707</v>
       </c>
       <c r="D14" t="n">
-        <v>1.17171874316707</v>
+        <v>0.241309995361339</v>
       </c>
       <c r="E14" t="n">
-        <v>0.241309995361339</v>
-      </c>
-      <c r="F14" t="n">
         <v>0.428275657868366</v>
       </c>
+      <c r="F14" t="s">
+        <v>58</v>
+      </c>
       <c r="G14" t="n">
-        <v>29.0506378211092</v>
-      </c>
-      <c r="H14" t="n">
         <v>3.52727671502126</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add BS_F0GNWEJJ to Table 2
</commit_message>
<xml_diff>
--- a/tables/results/TableS4-survival-results-table.xlsx
+++ b/tables/results/TableS4-survival-results-table.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t xml:space="preserve">term</t>
   </si>
@@ -115,85 +115,76 @@
     <t xml:space="preserve">hgg_groupHGG</t>
   </si>
   <si>
-    <t xml:space="preserve">1572945838334.15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2068.45013556778</t>
+    <t xml:space="preserve">B_cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.96219708727865e+55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macrophage_M1</t>
   </si>
   <si>
     <t xml:space="preserve">Inf</t>
   </si>
   <si>
-    <t xml:space="preserve">4.32242977898441</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B_cell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.60269538760554e+68</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrophage_M1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Macrophage_M2</t>
   </si>
   <si>
-    <t xml:space="preserve">1.35246231730248e+169</t>
+    <t xml:space="preserve">1.72448138540269e+157</t>
   </si>
   <si>
     <t xml:space="preserve">Monocyte</t>
   </si>
   <si>
-    <t xml:space="preserve">2.3484686232254e+30</t>
+    <t xml:space="preserve">1.17394365904452e+31</t>
   </si>
   <si>
     <t xml:space="preserve">Myeloid_dendritic_cell</t>
   </si>
   <si>
-    <t xml:space="preserve">1.06479257434283e+28</t>
+    <t xml:space="preserve">7.5450990381288e+27</t>
   </si>
   <si>
     <t xml:space="preserve">Neutrophil</t>
   </si>
   <si>
-    <t xml:space="preserve">1.50489322180708e+108</t>
+    <t xml:space="preserve">1.40507973230456e+96</t>
   </si>
   <si>
     <t xml:space="preserve">NK_cell</t>
   </si>
   <si>
-    <t xml:space="preserve">2823706437591606272</t>
+    <t xml:space="preserve">75389233841808080</t>
   </si>
   <si>
     <t xml:space="preserve">T_cell_CD4_non_regulatory</t>
   </si>
   <si>
-    <t xml:space="preserve">3.94583133618291e+46</t>
+    <t xml:space="preserve">1.37460054863856e+41</t>
   </si>
   <si>
     <t xml:space="preserve">T_cell_CD8</t>
   </si>
   <si>
-    <t xml:space="preserve">1.26769440002487e+103</t>
+    <t xml:space="preserve">7.85034422822238e+83</t>
   </si>
   <si>
     <t xml:space="preserve">T_cell_regulatory_Tregs</t>
   </si>
   <si>
-    <t xml:space="preserve">4.88417817394597e+131</t>
+    <t xml:space="preserve">4.45300383031584e+138</t>
   </si>
   <si>
     <t xml:space="preserve">CD274</t>
   </si>
   <si>
-    <t xml:space="preserve">0.18045003090112</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.60975614839146</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29.0506378211092</t>
+    <t xml:space="preserve">0.176248416339303</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.04209099445174</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.9748132155806</t>
   </si>
 </sst>
 </file>
@@ -553,22 +544,22 @@
         <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>0.47844633411542</v>
+        <v>0.465818347395348</v>
       </c>
       <c r="C2" t="n">
-        <v>1.26309420699082</v>
+        <v>1.0400023613673</v>
       </c>
       <c r="D2" t="n">
-        <v>0.206555325652364</v>
+        <v>0.298338803586208</v>
       </c>
       <c r="E2" t="n">
-        <v>0.716472946394793</v>
+        <v>0.651462787020435</v>
       </c>
       <c r="F2" t="n">
-        <v>4.67421099034643</v>
+        <v>4.0448293652004</v>
       </c>
       <c r="G2" t="n">
-        <v>1.83001249184929</v>
+        <v>1.62328549900366</v>
       </c>
     </row>
     <row r="3">
@@ -576,22 +567,22 @@
         <v>8</v>
       </c>
       <c r="B3" t="n">
-        <v>0.372657336884355</v>
+        <v>0.350700293353116</v>
       </c>
       <c r="C3" t="n">
-        <v>3.08578123504979</v>
+        <v>2.94849287703242</v>
       </c>
       <c r="D3" t="n">
-        <v>0.00203018130922217</v>
+        <v>0.00319327498369769</v>
       </c>
       <c r="E3" t="n">
-        <v>1.52126778819255</v>
+        <v>1.41436034033289</v>
       </c>
       <c r="F3" t="n">
-        <v>6.55569394190831</v>
+        <v>5.59233696356654</v>
       </c>
       <c r="G3" t="n">
-        <v>3.15800032030938</v>
+        <v>2.81239748453987</v>
       </c>
     </row>
     <row r="4">
@@ -599,22 +590,22 @@
         <v>9</v>
       </c>
       <c r="B4" t="n">
-        <v>0.475306896240576</v>
+        <v>0.467490340300323</v>
       </c>
       <c r="C4" t="n">
-        <v>-1.55535277919785</v>
+        <v>-1.8686182159355</v>
       </c>
       <c r="D4" t="n">
-        <v>0.119862073744265</v>
+        <v>0.0616759496058916</v>
       </c>
       <c r="E4" t="n">
-        <v>0.188086314793378</v>
+        <v>0.166989357562271</v>
       </c>
       <c r="F4" t="n">
-        <v>1.21205164266067</v>
+        <v>1.04362816732101</v>
       </c>
       <c r="G4" t="n">
-        <v>0.477462382609672</v>
+        <v>0.41746233027044</v>
       </c>
     </row>
     <row r="5">
@@ -622,22 +613,22 @@
         <v>10</v>
       </c>
       <c r="B5" t="n">
-        <v>0.461653149975373</v>
+        <v>0.448963153953435</v>
       </c>
       <c r="C5" t="n">
-        <v>0.703782189906269</v>
+        <v>0.488043133232366</v>
       </c>
       <c r="D5" t="n">
-        <v>0.481568426704985</v>
+        <v>0.625519289385329</v>
       </c>
       <c r="E5" t="n">
-        <v>0.55994300207926</v>
+        <v>0.516418276874473</v>
       </c>
       <c r="F5" t="n">
-        <v>3.42029502566414</v>
+        <v>3.00135843094532</v>
       </c>
       <c r="G5" t="n">
-        <v>1.38389676806731</v>
+        <v>1.24497242908887</v>
       </c>
     </row>
   </sheetData>
@@ -691,31 +682,31 @@
         <v>21</v>
       </c>
       <c r="B2" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C2" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D2" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E2" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F2" t="n">
-        <v>615.461538461538</v>
+        <v>563.733333333333</v>
       </c>
       <c r="G2" t="n">
-        <v>96.9345912198832</v>
+        <v>91.9978969163809</v>
       </c>
       <c r="H2" t="n">
-        <v>536</v>
+        <v>400</v>
       </c>
       <c r="I2" t="n">
         <v>355</v>
       </c>
-      <c r="J2" t="e">
-        <v>#N/A</v>
+      <c r="J2" t="n">
+        <v>854</v>
       </c>
     </row>
     <row r="3">
@@ -755,31 +746,31 @@
         <v>23</v>
       </c>
       <c r="B4" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C4" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D4" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E4" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F4" t="n">
-        <v>302.346153846154</v>
+        <v>292.518518518519</v>
       </c>
       <c r="G4" t="n">
-        <v>26.2542722535061</v>
+        <v>27.0588126602017</v>
       </c>
       <c r="H4" t="n">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="I4" t="n">
         <v>244</v>
       </c>
       <c r="J4" t="n">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="5">
@@ -888,22 +879,22 @@
         <v>26</v>
       </c>
       <c r="B2" t="n">
-        <v>0.454121173826659</v>
+        <v>0.415323156973027</v>
       </c>
       <c r="C2" t="n">
-        <v>1.4647217127197</v>
+        <v>0.69784038235957</v>
       </c>
       <c r="D2" t="n">
-        <v>0.142996858543784</v>
+        <v>0.485277021551417</v>
       </c>
       <c r="E2" t="n">
-        <v>0.798596072930393</v>
+        <v>0.592035216256427</v>
       </c>
       <c r="F2" t="n">
-        <v>4.73613919898317</v>
+        <v>3.0157474209742</v>
       </c>
       <c r="G2" t="n">
-        <v>1.94480388861182</v>
+        <v>1.33619934012528</v>
       </c>
     </row>
     <row r="3">
@@ -911,22 +902,22 @@
         <v>27</v>
       </c>
       <c r="B3" t="n">
-        <v>0.614572617817878</v>
+        <v>0.579918080622965</v>
       </c>
       <c r="C3" t="n">
-        <v>5.14512973859145</v>
+        <v>5.16794023799259</v>
       </c>
       <c r="D3" t="n">
-        <v>0.000000267335988648007</v>
+        <v>0.000000236687961194656</v>
       </c>
       <c r="E3" t="n">
-        <v>7.08171178235642</v>
+        <v>6.42607178455667</v>
       </c>
       <c r="F3" t="n">
-        <v>78.7750284868543</v>
+        <v>62.4022002765239</v>
       </c>
       <c r="G3" t="n">
-        <v>23.6191034417232</v>
+        <v>20.025009824997</v>
       </c>
     </row>
     <row r="4">
@@ -934,22 +925,22 @@
         <v>28</v>
       </c>
       <c r="B4" t="n">
-        <v>0.312839353936692</v>
+        <v>0.294691093498945</v>
       </c>
       <c r="C4" t="n">
-        <v>-3.23105079323403</v>
+        <v>-3.57166001832015</v>
       </c>
       <c r="D4" t="n">
-        <v>0.00123336020308562</v>
+        <v>0.000354725708053518</v>
       </c>
       <c r="E4" t="n">
-        <v>0.197117809867498</v>
+        <v>0.195906000078641</v>
       </c>
       <c r="F4" t="n">
-        <v>0.671899854215695</v>
+        <v>0.621914617489566</v>
       </c>
       <c r="G4" t="n">
-        <v>0.363927778155624</v>
+        <v>0.349051292939618</v>
       </c>
     </row>
     <row r="5">
@@ -957,22 +948,22 @@
         <v>29</v>
       </c>
       <c r="B5" t="n">
-        <v>0.299884699761876</v>
+        <v>0.289489434667261</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.85925192801687</v>
+        <v>-1.23861996630689</v>
       </c>
       <c r="D5" t="n">
-        <v>0.390201539716764</v>
+        <v>0.215486270336434</v>
       </c>
       <c r="E5" t="n">
-        <v>0.429368515844325</v>
+        <v>0.396152413315291</v>
       </c>
       <c r="F5" t="n">
-        <v>1.39108873702023</v>
+        <v>1.23222499227675</v>
       </c>
       <c r="G5" t="n">
-        <v>0.772845202108501</v>
+        <v>0.698676537775422</v>
       </c>
     </row>
     <row r="6">
@@ -980,22 +971,22 @@
         <v>30</v>
       </c>
       <c r="B6" t="n">
-        <v>1.02177506179121</v>
+        <v>1.02019354504279</v>
       </c>
       <c r="C6" t="n">
-        <v>-2.63589644753672</v>
+        <v>-3.01787456266425</v>
       </c>
       <c r="D6" t="n">
-        <v>0.00839153358374639</v>
+        <v>0.00254554246690893</v>
       </c>
       <c r="E6" t="n">
-        <v>0.00913231938217678</v>
+        <v>0.0062301257978024</v>
       </c>
       <c r="F6" t="n">
-        <v>0.501249682315998</v>
+        <v>0.339842316810626</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0676577577896604</v>
+        <v>0.0460136977990991</v>
       </c>
     </row>
     <row r="7">
@@ -1003,22 +994,22 @@
         <v>31</v>
       </c>
       <c r="B7" t="n">
-        <v>0.237798791317952</v>
+        <v>0.22050713531354</v>
       </c>
       <c r="C7" t="n">
-        <v>7.28355277926011</v>
+        <v>8.24003617258086</v>
       </c>
       <c r="D7" t="n">
-        <v>0.000000000000325141633705587</v>
+        <v>0.000000000000000172158598720108</v>
       </c>
       <c r="E7" t="n">
-        <v>3.54643538051519</v>
+        <v>3.99402992616956</v>
       </c>
       <c r="F7" t="n">
-        <v>9.00785625654152</v>
+        <v>9.47989096714135</v>
       </c>
       <c r="G7" t="n">
-        <v>5.65205981309416</v>
+        <v>6.15328921956274</v>
       </c>
     </row>
   </sheetData>
@@ -1063,22 +1054,22 @@
         <v>26</v>
       </c>
       <c r="B2" t="n">
-        <v>2.64087618039762</v>
+        <v>2.70833398718874</v>
       </c>
       <c r="C2" t="n">
-        <v>2.79648917502214</v>
+        <v>2.80703632720436</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0051661141554533</v>
+        <v>0.00499996028205463</v>
       </c>
       <c r="E2" t="n">
-        <v>9.10805739556573</v>
+        <v>9.91605157396784</v>
       </c>
       <c r="F2" t="n">
-        <v>285273.558212938</v>
+        <v>404589.787021872</v>
       </c>
       <c r="G2" t="n">
-        <v>1611.92057547532</v>
+        <v>2002.98107689752</v>
       </c>
     </row>
     <row r="3">
@@ -1086,22 +1077,22 @@
         <v>27</v>
       </c>
       <c r="B3" t="n">
-        <v>7.32532067488232</v>
+        <v>7.81287790461211</v>
       </c>
       <c r="C3" t="n">
-        <v>3.02805248573249</v>
+        <v>2.97994007202059</v>
       </c>
       <c r="D3" t="n">
-        <v>0.00246135333921797</v>
+        <v>0.00288304780223201</v>
       </c>
       <c r="E3" t="n">
-        <v>2500.11192633725</v>
+        <v>2889.81751960963</v>
       </c>
       <c r="F3" t="n">
-        <v>7389379609457043</v>
+        <v>57748123738393616</v>
       </c>
       <c r="G3" t="n">
-        <v>4298171249.47772</v>
+        <v>12918263803.77</v>
       </c>
     </row>
     <row r="4">
@@ -1109,22 +1100,22 @@
         <v>28</v>
       </c>
       <c r="B4" t="n">
-        <v>1.37753051015512</v>
+        <v>1.45568588735954</v>
       </c>
       <c r="C4" t="n">
-        <v>-20.959587102819</v>
+        <v>-20.1250974336236</v>
       </c>
       <c r="D4" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000153412046828091</v>
+        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000444896745525201</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0000000000000194217873077806</v>
+        <v>0.0000000000000109120116313269</v>
       </c>
       <c r="F4" t="n">
-        <v>0.00000000000429933598658414</v>
+        <v>0.00000000000328147400131446</v>
       </c>
       <c r="G4" t="n">
-        <v>0.000000000000288965030922644</v>
+        <v>0.000000000000189228651293192</v>
       </c>
     </row>
     <row r="5">
@@ -1192,22 +1183,22 @@
         <v>26</v>
       </c>
       <c r="B2" t="n">
-        <v>6.98979694342947</v>
+        <v>3.97293432439853</v>
       </c>
       <c r="C2" t="n">
-        <v>2.05788825560674</v>
+        <v>2.20733773406908</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0396008613847964</v>
+        <v>0.0272904729423655</v>
       </c>
       <c r="E2" t="n">
-        <v>1.98272224290025</v>
-      </c>
-      <c r="F2" t="s">
-        <v>32</v>
+        <v>2.67192626660192</v>
+      </c>
+      <c r="F2" t="n">
+        <v>15501014.6027207</v>
       </c>
       <c r="G2" t="n">
-        <v>1765988.30702315</v>
+        <v>6435.64822500339</v>
       </c>
     </row>
     <row r="3">
@@ -1215,22 +1206,22 @@
         <v>27</v>
       </c>
       <c r="B3" t="n">
-        <v>4.00301291683135</v>
+        <v>3.2672842309817</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.0527618251505884</v>
+        <v>0.369239995928948</v>
       </c>
       <c r="D3" t="n">
-        <v>0.957921678227888</v>
+        <v>0.71194884644948</v>
       </c>
       <c r="E3" t="n">
-        <v>0.000316886334627329</v>
-      </c>
-      <c r="F3" t="s">
-        <v>33</v>
+        <v>0.0055312170635766</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2018.62413315608</v>
       </c>
       <c r="G3" t="n">
-        <v>0.80960705395857</v>
+        <v>3.34147396372626</v>
       </c>
     </row>
     <row r="4">
@@ -1238,22 +1229,22 @@
         <v>28</v>
       </c>
       <c r="B4" t="n">
-        <v>15663.1915129564</v>
+        <v>2.0757041261229</v>
       </c>
       <c r="C4" t="n">
-        <v>0.00143963573978737</v>
+        <v>2.7142576358903</v>
       </c>
       <c r="D4" t="n">
-        <v>0.998851337266821</v>
+        <v>0.00664244850422233</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="s">
-        <v>34</v>
+        <v>4.78597824734361</v>
+      </c>
+      <c r="F4" t="n">
+        <v>16355.1989429013</v>
       </c>
       <c r="G4" t="n">
-        <v>6209152816.90122</v>
+        <v>279.77781608216</v>
       </c>
     </row>
     <row r="5">
@@ -1261,22 +1252,22 @@
         <v>29</v>
       </c>
       <c r="B5" t="n">
-        <v>0.693887226261366</v>
+        <v>0.617902375881565</v>
       </c>
       <c r="C5" t="n">
-        <v>0.149626216258029</v>
+        <v>0.427980317828389</v>
       </c>
       <c r="D5" t="n">
-        <v>0.881059523440836</v>
+        <v>0.668665450085559</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2847424325918</v>
-      </c>
-      <c r="F5" t="s">
-        <v>35</v>
+        <v>0.38805183711419</v>
+      </c>
+      <c r="F5" t="n">
+        <v>4.3732938119543</v>
       </c>
       <c r="G5" t="n">
-        <v>1.10940487198104</v>
+        <v>1.30271435778109</v>
       </c>
     </row>
   </sheetData>
@@ -1318,45 +1309,45 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B2" t="n">
-        <v>65.9451574467056</v>
+        <v>61.646351528879</v>
       </c>
       <c r="C2" t="n">
-        <v>0.447003684362564</v>
+        <v>0.131659843232311</v>
       </c>
       <c r="D2" t="n">
-        <v>0.654872399695274</v>
+        <v>0.895253349399446</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0000000000000000000000000000000000000000000467083980799242</v>
+        <v>0.0000000000000000000000000000000000000000000000001125682771932</v>
       </c>
       <c r="F2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G2" t="n">
-        <v>6338912530746.95</v>
+        <v>3348.77195875451</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B3" t="n">
-        <v>24841596.4241147</v>
+        <v>38323732.4486327</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.00360331808662127</v>
+        <v>-0.00258440917112054</v>
       </c>
       <c r="D3" t="n">
-        <v>0.997124974352533</v>
+        <v>0.997937942119039</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -1364,209 +1355,209 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B4" t="n">
-        <v>157.972414593224</v>
+        <v>153.700235842784</v>
       </c>
       <c r="C4" t="n">
-        <v>0.505269003058629</v>
+        <v>0.395600299235897</v>
       </c>
       <c r="D4" t="n">
-        <v>0.613369910816791</v>
+        <v>0.692399916315753</v>
       </c>
       <c r="E4" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000157906133407611</v>
+        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000377487545173725</v>
       </c>
       <c r="F4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G4" t="n">
-        <v>46212779088120034539933417387065344</v>
+        <v>255141185400050386768756736</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B5" t="n">
-        <v>14.8633057493278</v>
+        <v>14.9714869453789</v>
       </c>
       <c r="C5" t="n">
-        <v>2.74499986638744</v>
+        <v>2.81848633729382</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0060510922336591</v>
+        <v>0.00482506644640399</v>
       </c>
       <c r="E5" t="n">
-        <v>116801.166454098</v>
+        <v>382068.8842405</v>
       </c>
       <c r="F5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G5" t="n">
-        <v>523740273965613504</v>
+        <v>2117846415518244864</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B6" t="n">
-        <v>23.5766860637712</v>
+        <v>23.9561745009308</v>
       </c>
       <c r="C6" t="n">
-        <v>0.777280870126654</v>
+        <v>0.719541281495004</v>
       </c>
       <c r="D6" t="n">
-        <v>0.436993078868274</v>
+        <v>0.471807476334453</v>
       </c>
       <c r="E6" t="n">
-        <v>0.00000000000077667958706768</v>
+        <v>0.000000000000124336756882828</v>
       </c>
       <c r="F6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G6" t="n">
-        <v>90939686.4385031</v>
+        <v>30628959.2503676</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B7" t="n">
-        <v>116.600571810765</v>
+        <v>81.5462546620844</v>
       </c>
       <c r="C7" t="n">
-        <v>0.176285504822041</v>
+        <v>0.754915612260259</v>
       </c>
       <c r="D7" t="n">
-        <v>0.860069649178577</v>
+        <v>0.450299617579022</v>
       </c>
       <c r="E7" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000474605051084553</v>
+        <v>0.000000000000000000000000000000000000000000210428881025276</v>
       </c>
       <c r="F7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G7" t="n">
-        <v>845121248.349933</v>
+        <v>543754867399032139587518464</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B8" t="n">
-        <v>30.8115155144595</v>
+        <v>31.6576285786488</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.58110996434463</v>
+        <v>-0.732410228391202</v>
       </c>
       <c r="D8" t="n">
-        <v>0.5611663434077</v>
+        <v>0.463918217624204</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0000000000000000000000000000000000993574494765512</v>
+        <v>0.0000000000000000000000000000000000000962198617114453</v>
       </c>
       <c r="F8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0000000167498140201503</v>
+        <v>0.0000000000851700748783902</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B9" t="n">
-        <v>34.5465361079373</v>
+        <v>33.8261667896644</v>
       </c>
       <c r="C9" t="n">
-        <v>1.14574749999797</v>
+        <v>0.840357807183923</v>
       </c>
       <c r="D9" t="n">
-        <v>0.25189964364869</v>
+        <v>0.40070779861187</v>
       </c>
       <c r="E9" t="n">
-        <v>0.000000000000608147354514014</v>
+        <v>0.0000000000000000356784326903035</v>
       </c>
       <c r="F9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G9" t="n">
-        <v>154907936803062144</v>
+        <v>2214578812114.3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B10" t="n">
-        <v>164.855190435033</v>
+        <v>167.242428728349</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.5198912530147</v>
+        <v>-0.804903503961642</v>
       </c>
       <c r="D10" t="n">
-        <v>0.603139372257192</v>
+        <v>0.420875366242144</v>
       </c>
       <c r="E10" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000283811220481693</v>
+        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000151656787184261</v>
       </c>
       <c r="F10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0000000000000000000000000000000000000599821552521129</v>
+        <v>0.0000000000000000000000000000000000000000000000000000000000345044632466977</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B11" t="n">
-        <v>207.873606394647</v>
+        <v>207.962366767297</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.50126678157103</v>
+        <v>-0.424828918122422</v>
       </c>
       <c r="D11" t="n">
-        <v>0.616183380381179</v>
+        <v>0.670961395180726</v>
       </c>
       <c r="E11" t="n">
-        <v>6.36974996404952e-223</v>
+        <v>4.10088908077937e-216</v>
       </c>
       <c r="F11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G11" t="n">
-        <v>0.000000000000000000000000000000000000000000000557772298952752</v>
+        <v>0.00000000000000000000000000000000000000427332128261039</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B12" t="n">
-        <v>2.80418927214936</v>
+        <v>2.56641039744572</v>
       </c>
       <c r="C12" t="n">
-        <v>-2.57058659609299</v>
+        <v>-2.63634092891602</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0101526440656152</v>
+        <v>0.00838054830599798</v>
       </c>
       <c r="E12" t="n">
-        <v>0.00000303736153615593</v>
+        <v>0.00000753460070200555</v>
       </c>
       <c r="F12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G12" t="n">
-        <v>0.000740332346353454</v>
+        <v>0.0011523720933264</v>
       </c>
     </row>
     <row r="13">
@@ -1574,22 +1565,22 @@
         <v>28</v>
       </c>
       <c r="B13" t="n">
-        <v>1.0951663933398</v>
+        <v>1.08929723803791</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.235525786517619</v>
+        <v>-0.308669847036519</v>
       </c>
       <c r="D13" t="n">
-        <v>0.813800666948844</v>
+        <v>0.757572683059894</v>
       </c>
       <c r="E13" t="n">
-        <v>0.0903172674058606</v>
+        <v>0.084482018434504</v>
       </c>
       <c r="F13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G13" t="n">
-        <v>0.772641646264168</v>
+        <v>0.714456466676748</v>
       </c>
     </row>
     <row r="14">
@@ -1597,22 +1588,22 @@
         <v>29</v>
       </c>
       <c r="B14" t="n">
-        <v>1.07579238765984</v>
+        <v>1.06674239484188</v>
       </c>
       <c r="C14" t="n">
-        <v>1.17171874316707</v>
+        <v>1.09337612997911</v>
       </c>
       <c r="D14" t="n">
-        <v>0.241309995361339</v>
+        <v>0.274228689512069</v>
       </c>
       <c r="E14" t="n">
-        <v>0.428275657868366</v>
+        <v>0.396759092130491</v>
       </c>
       <c r="F14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G14" t="n">
-        <v>3.52727671502126</v>
+        <v>3.21025595703409</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated table S2 to  have a table of all primary_only oncoprint alterations, re-ran module
</commit_message>
<xml_diff>
--- a/tables/results/TableS4-survival-results-table.xlsx
+++ b/tables/results/TableS4-survival-results-table.xlsx
@@ -118,7 +118,7 @@
     <t xml:space="preserve">B_cell</t>
   </si>
   <si>
-    <t xml:space="preserve">9.96219708727865e+55</t>
+    <t xml:space="preserve">9.96219708727837e+55</t>
   </si>
   <si>
     <t xml:space="preserve">Macrophage_M1</t>
@@ -130,7 +130,7 @@
     <t xml:space="preserve">Macrophage_M2</t>
   </si>
   <si>
-    <t xml:space="preserve">1.72448138540269e+157</t>
+    <t xml:space="preserve">1.72448138540289e+157</t>
   </si>
   <si>
     <t xml:space="preserve">Monocyte</t>
@@ -148,7 +148,7 @@
     <t xml:space="preserve">Neutrophil</t>
   </si>
   <si>
-    <t xml:space="preserve">1.40507973230456e+96</t>
+    <t xml:space="preserve">1.40507973230373e+96</t>
   </si>
   <si>
     <t xml:space="preserve">NK_cell</t>
@@ -160,31 +160,31 @@
     <t xml:space="preserve">T_cell_CD4_non_regulatory</t>
   </si>
   <si>
-    <t xml:space="preserve">1.37460054863856e+41</t>
+    <t xml:space="preserve">1.37460054863858e+41</t>
   </si>
   <si>
     <t xml:space="preserve">T_cell_CD8</t>
   </si>
   <si>
-    <t xml:space="preserve">7.85034422822238e+83</t>
+    <t xml:space="preserve">7.85034422822483e+83</t>
   </si>
   <si>
     <t xml:space="preserve">T_cell_regulatory_Tregs</t>
   </si>
   <si>
-    <t xml:space="preserve">4.45300383031584e+138</t>
+    <t xml:space="preserve">4.45300383031963e+138</t>
   </si>
   <si>
     <t xml:space="preserve">CD274</t>
   </si>
   <si>
-    <t xml:space="preserve">0.176248416339303</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.04209099445174</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25.9748132155806</t>
+    <t xml:space="preserve">0.176248416339304</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.04209099445168</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.9748132155803</t>
   </si>
 </sst>
 </file>
@@ -544,22 +544,22 @@
         <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>0.465818347395348</v>
+        <v>0.460705037119029</v>
       </c>
       <c r="C2" t="n">
-        <v>1.0400023613673</v>
+        <v>0.916373721657586</v>
       </c>
       <c r="D2" t="n">
-        <v>0.298338803586208</v>
+        <v>0.359470913310476</v>
       </c>
       <c r="E2" t="n">
-        <v>0.651462787020435</v>
+        <v>0.618296421054565</v>
       </c>
       <c r="F2" t="n">
-        <v>4.0448293652004</v>
+        <v>3.76272440078304</v>
       </c>
       <c r="G2" t="n">
-        <v>1.62328549900366</v>
+        <v>1.52527998427136</v>
       </c>
     </row>
     <row r="3">
@@ -567,22 +567,22 @@
         <v>8</v>
       </c>
       <c r="B3" t="n">
-        <v>0.350700293353116</v>
+        <v>0.340620087855469</v>
       </c>
       <c r="C3" t="n">
-        <v>2.94849287703242</v>
+        <v>2.87287553384664</v>
       </c>
       <c r="D3" t="n">
-        <v>0.00319327498369769</v>
+        <v>0.00406754333009253</v>
       </c>
       <c r="E3" t="n">
-        <v>1.41436034033289</v>
+        <v>1.36472918833444</v>
       </c>
       <c r="F3" t="n">
-        <v>5.59233696356654</v>
+        <v>5.18703488774961</v>
       </c>
       <c r="G3" t="n">
-        <v>2.81239748453987</v>
+        <v>2.66061983609476</v>
       </c>
     </row>
     <row r="4">
@@ -590,22 +590,22 @@
         <v>9</v>
       </c>
       <c r="B4" t="n">
-        <v>0.467490340300323</v>
+        <v>0.463023356211318</v>
       </c>
       <c r="C4" t="n">
-        <v>-1.8686182159355</v>
+        <v>-1.99769413663694</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0616759496058916</v>
+        <v>0.0457498302823641</v>
       </c>
       <c r="E4" t="n">
-        <v>0.166989357562271</v>
+        <v>0.160014931535711</v>
       </c>
       <c r="F4" t="n">
-        <v>1.04362816732101</v>
+        <v>0.982681773009629</v>
       </c>
       <c r="G4" t="n">
-        <v>0.41746233027044</v>
+        <v>0.396539728942166</v>
       </c>
     </row>
     <row r="5">
@@ -613,22 +613,22 @@
         <v>10</v>
       </c>
       <c r="B5" t="n">
-        <v>0.448963153953435</v>
+        <v>0.443914033175195</v>
       </c>
       <c r="C5" t="n">
-        <v>0.488043133232366</v>
+        <v>0.353812613740699</v>
       </c>
       <c r="D5" t="n">
-        <v>0.625519289385329</v>
+        <v>0.72347931979534</v>
       </c>
       <c r="E5" t="n">
-        <v>0.516418276874473</v>
+        <v>0.490174841124133</v>
       </c>
       <c r="F5" t="n">
-        <v>3.00135843094532</v>
+        <v>2.79300450971034</v>
       </c>
       <c r="G5" t="n">
-        <v>1.24497242908887</v>
+        <v>1.17006860559809</v>
       </c>
     </row>
   </sheetData>
@@ -682,28 +682,28 @@
         <v>21</v>
       </c>
       <c r="B2" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F2" t="n">
-        <v>563.733333333333</v>
+        <v>539.6875</v>
       </c>
       <c r="G2" t="n">
-        <v>91.9978969163809</v>
+        <v>89.3352498470474</v>
       </c>
       <c r="H2" t="n">
-        <v>400</v>
+        <v>399.5</v>
       </c>
       <c r="I2" t="n">
-        <v>355</v>
+        <v>336</v>
       </c>
       <c r="J2" t="n">
         <v>854</v>
@@ -746,28 +746,28 @@
         <v>23</v>
       </c>
       <c r="B4" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C4" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D4" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E4" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F4" t="n">
-        <v>292.518518518519</v>
+        <v>287.035714285714</v>
       </c>
       <c r="G4" t="n">
-        <v>27.0588126602017</v>
+        <v>26.6421142247463</v>
       </c>
       <c r="H4" t="n">
-        <v>274</v>
+        <v>273.5</v>
       </c>
       <c r="I4" t="n">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="J4" t="n">
         <v>392</v>
@@ -1312,22 +1312,22 @@
         <v>32</v>
       </c>
       <c r="B2" t="n">
-        <v>61.646351528879</v>
+        <v>61.6463515288789</v>
       </c>
       <c r="C2" t="n">
-        <v>0.131659843232311</v>
+        <v>0.131659843232312</v>
       </c>
       <c r="D2" t="n">
         <v>0.895253349399446</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0000000000000000000000000000000000000000000000001125682771932</v>
+        <v>0.000000000000000000000000000000000000000000000000112568277193212</v>
       </c>
       <c r="F2" t="s">
         <v>33</v>
       </c>
       <c r="G2" t="n">
-        <v>3348.77195875451</v>
+        <v>3348.77195875469</v>
       </c>
     </row>
     <row r="3">
@@ -1335,13 +1335,13 @@
         <v>34</v>
       </c>
       <c r="B3" t="n">
-        <v>38323732.4486327</v>
+        <v>38323732.5619672</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.00258440917112054</v>
+        <v>-0.00258440916592485</v>
       </c>
       <c r="D3" t="n">
-        <v>0.997937942119039</v>
+        <v>0.997937942123184</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -1361,19 +1361,19 @@
         <v>153.700235842784</v>
       </c>
       <c r="C4" t="n">
-        <v>0.395600299235897</v>
+        <v>0.395600299235896</v>
       </c>
       <c r="D4" t="n">
-        <v>0.692399916315753</v>
+        <v>0.692399916315754</v>
       </c>
       <c r="E4" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000377487545173725</v>
+        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000377487545173532</v>
       </c>
       <c r="F4" t="s">
         <v>37</v>
       </c>
       <c r="G4" t="n">
-        <v>255141185400050386768756736</v>
+        <v>255141185400005066273849344</v>
       </c>
     </row>
     <row r="5">
@@ -1387,16 +1387,16 @@
         <v>2.81848633729382</v>
       </c>
       <c r="D5" t="n">
-        <v>0.00482506644640399</v>
+        <v>0.00482506644640395</v>
       </c>
       <c r="E5" t="n">
-        <v>382068.8842405</v>
+        <v>382068.884240511</v>
       </c>
       <c r="F5" t="s">
         <v>39</v>
       </c>
       <c r="G5" t="n">
-        <v>2117846415518244864</v>
+        <v>2117846415518274816</v>
       </c>
     </row>
     <row r="6">
@@ -1407,19 +1407,19 @@
         <v>23.9561745009308</v>
       </c>
       <c r="C6" t="n">
-        <v>0.719541281495004</v>
+        <v>0.719541281495003</v>
       </c>
       <c r="D6" t="n">
-        <v>0.471807476334453</v>
+        <v>0.471807476334454</v>
       </c>
       <c r="E6" t="n">
-        <v>0.000000000000124336756882828</v>
+        <v>0.000000000000124336756882823</v>
       </c>
       <c r="F6" t="s">
         <v>41</v>
       </c>
       <c r="G6" t="n">
-        <v>30628959.2503676</v>
+        <v>30628959.2503669</v>
       </c>
     </row>
     <row r="7">
@@ -1427,22 +1427,22 @@
         <v>42</v>
       </c>
       <c r="B7" t="n">
-        <v>81.5462546620844</v>
+        <v>81.5462546620843</v>
       </c>
       <c r="C7" t="n">
-        <v>0.754915612260259</v>
+        <v>0.754915612260255</v>
       </c>
       <c r="D7" t="n">
-        <v>0.450299617579022</v>
+        <v>0.450299617579024</v>
       </c>
       <c r="E7" t="n">
-        <v>0.000000000000000000000000000000000000000000210428881025276</v>
+        <v>0.000000000000000000000000000000000000000000210428881025237</v>
       </c>
       <c r="F7" t="s">
         <v>43</v>
       </c>
       <c r="G7" t="n">
-        <v>543754867399032139587518464</v>
+        <v>543754867398827355546845184</v>
       </c>
     </row>
     <row r="8">
@@ -1450,22 +1450,22 @@
         <v>44</v>
       </c>
       <c r="B8" t="n">
-        <v>31.6576285786488</v>
+        <v>31.6576285786489</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.732410228391202</v>
+        <v>-0.732410228391203</v>
       </c>
       <c r="D8" t="n">
         <v>0.463918217624204</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0000000000000000000000000000000000000962198617114453</v>
+        <v>0.000000000000000000000000000000000000096219861711433</v>
       </c>
       <c r="F8" t="s">
         <v>45</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0000000000851700748783902</v>
+        <v>0.0000000000851700748783847</v>
       </c>
     </row>
     <row r="9">
@@ -1476,19 +1476,19 @@
         <v>33.8261667896644</v>
       </c>
       <c r="C9" t="n">
-        <v>0.840357807183923</v>
+        <v>0.840357807183922</v>
       </c>
       <c r="D9" t="n">
-        <v>0.40070779861187</v>
+        <v>0.400707798611871</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0000000000000000356784326903035</v>
+        <v>0.000000000000000035678432690302</v>
       </c>
       <c r="F9" t="s">
         <v>47</v>
       </c>
       <c r="G9" t="n">
-        <v>2214578812114.3</v>
+        <v>2214578812114.25</v>
       </c>
     </row>
     <row r="10">
@@ -1499,19 +1499,19 @@
         <v>167.242428728349</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.804903503961642</v>
+        <v>-0.80490350396164</v>
       </c>
       <c r="D10" t="n">
-        <v>0.420875366242144</v>
+        <v>0.420875366242145</v>
       </c>
       <c r="E10" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000151656787184261</v>
+        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000151656787184304</v>
       </c>
       <c r="F10" t="s">
         <v>49</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000345044632466977</v>
+        <v>0.0000000000000000000000000000000000000000000000000000000000345044632467085</v>
       </c>
     </row>
     <row r="11">
@@ -1522,19 +1522,19 @@
         <v>207.962366767297</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.424828918122422</v>
+        <v>-0.424828918122417</v>
       </c>
       <c r="D11" t="n">
-        <v>0.670961395180726</v>
+        <v>0.67096139518073</v>
       </c>
       <c r="E11" t="n">
-        <v>4.10088908077937e-216</v>
+        <v>4.1008890807866e-216</v>
       </c>
       <c r="F11" t="s">
         <v>51</v>
       </c>
       <c r="G11" t="n">
-        <v>0.00000000000000000000000000000000000000427332128261039</v>
+        <v>0.00000000000000000000000000000000000000427332128261592</v>
       </c>
     </row>
     <row r="12">
@@ -1548,10 +1548,10 @@
         <v>-2.63634092891602</v>
       </c>
       <c r="D12" t="n">
-        <v>0.00838054830599798</v>
+        <v>0.00838054830599803</v>
       </c>
       <c r="E12" t="n">
-        <v>0.00000753460070200555</v>
+        <v>0.00000753460070200553</v>
       </c>
       <c r="F12" t="s">
         <v>53</v>
@@ -1565,16 +1565,16 @@
         <v>28</v>
       </c>
       <c r="B13" t="n">
-        <v>1.08929723803791</v>
+        <v>1.0892972380379</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.308669847036519</v>
+        <v>-0.30866984703652</v>
       </c>
       <c r="D13" t="n">
-        <v>0.757572683059894</v>
+        <v>0.757572683059893</v>
       </c>
       <c r="E13" t="n">
-        <v>0.084482018434504</v>
+        <v>0.084482018434505</v>
       </c>
       <c r="F13" t="s">
         <v>54</v>
@@ -1588,16 +1588,16 @@
         <v>29</v>
       </c>
       <c r="B14" t="n">
-        <v>1.06674239484188</v>
+        <v>1.06674239484187</v>
       </c>
       <c r="C14" t="n">
-        <v>1.09337612997911</v>
+        <v>1.09337612997912</v>
       </c>
       <c r="D14" t="n">
-        <v>0.274228689512069</v>
+        <v>0.274228689512066</v>
       </c>
       <c r="E14" t="n">
-        <v>0.396759092130491</v>
+        <v>0.396759092130496</v>
       </c>
       <c r="F14" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
Updated table S2 with oncoprint alterations (#1689)
* Updated table S2 to  have a table of all primary_only oncoprint alterations, re-ran module

* remove cache file

* Ensure there are no all-NA columns, and include 2023
</commit_message>
<xml_diff>
--- a/tables/results/TableS4-survival-results-table.xlsx
+++ b/tables/results/TableS4-survival-results-table.xlsx
@@ -118,7 +118,7 @@
     <t xml:space="preserve">B_cell</t>
   </si>
   <si>
-    <t xml:space="preserve">9.96219708727865e+55</t>
+    <t xml:space="preserve">9.96219708727837e+55</t>
   </si>
   <si>
     <t xml:space="preserve">Macrophage_M1</t>
@@ -130,7 +130,7 @@
     <t xml:space="preserve">Macrophage_M2</t>
   </si>
   <si>
-    <t xml:space="preserve">1.72448138540269e+157</t>
+    <t xml:space="preserve">1.72448138540289e+157</t>
   </si>
   <si>
     <t xml:space="preserve">Monocyte</t>
@@ -148,7 +148,7 @@
     <t xml:space="preserve">Neutrophil</t>
   </si>
   <si>
-    <t xml:space="preserve">1.40507973230456e+96</t>
+    <t xml:space="preserve">1.40507973230373e+96</t>
   </si>
   <si>
     <t xml:space="preserve">NK_cell</t>
@@ -160,31 +160,31 @@
     <t xml:space="preserve">T_cell_CD4_non_regulatory</t>
   </si>
   <si>
-    <t xml:space="preserve">1.37460054863856e+41</t>
+    <t xml:space="preserve">1.37460054863858e+41</t>
   </si>
   <si>
     <t xml:space="preserve">T_cell_CD8</t>
   </si>
   <si>
-    <t xml:space="preserve">7.85034422822238e+83</t>
+    <t xml:space="preserve">7.85034422822483e+83</t>
   </si>
   <si>
     <t xml:space="preserve">T_cell_regulatory_Tregs</t>
   </si>
   <si>
-    <t xml:space="preserve">4.45300383031584e+138</t>
+    <t xml:space="preserve">4.45300383031963e+138</t>
   </si>
   <si>
     <t xml:space="preserve">CD274</t>
   </si>
   <si>
-    <t xml:space="preserve">0.176248416339303</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.04209099445174</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25.9748132155806</t>
+    <t xml:space="preserve">0.176248416339304</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.04209099445168</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.9748132155803</t>
   </si>
 </sst>
 </file>
@@ -544,22 +544,22 @@
         <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>0.465818347395348</v>
+        <v>0.460705037119029</v>
       </c>
       <c r="C2" t="n">
-        <v>1.0400023613673</v>
+        <v>0.916373721657586</v>
       </c>
       <c r="D2" t="n">
-        <v>0.298338803586208</v>
+        <v>0.359470913310476</v>
       </c>
       <c r="E2" t="n">
-        <v>0.651462787020435</v>
+        <v>0.618296421054565</v>
       </c>
       <c r="F2" t="n">
-        <v>4.0448293652004</v>
+        <v>3.76272440078304</v>
       </c>
       <c r="G2" t="n">
-        <v>1.62328549900366</v>
+        <v>1.52527998427136</v>
       </c>
     </row>
     <row r="3">
@@ -567,22 +567,22 @@
         <v>8</v>
       </c>
       <c r="B3" t="n">
-        <v>0.350700293353116</v>
+        <v>0.340620087855469</v>
       </c>
       <c r="C3" t="n">
-        <v>2.94849287703242</v>
+        <v>2.87287553384664</v>
       </c>
       <c r="D3" t="n">
-        <v>0.00319327498369769</v>
+        <v>0.00406754333009253</v>
       </c>
       <c r="E3" t="n">
-        <v>1.41436034033289</v>
+        <v>1.36472918833444</v>
       </c>
       <c r="F3" t="n">
-        <v>5.59233696356654</v>
+        <v>5.18703488774961</v>
       </c>
       <c r="G3" t="n">
-        <v>2.81239748453987</v>
+        <v>2.66061983609476</v>
       </c>
     </row>
     <row r="4">
@@ -590,22 +590,22 @@
         <v>9</v>
       </c>
       <c r="B4" t="n">
-        <v>0.467490340300323</v>
+        <v>0.463023356211318</v>
       </c>
       <c r="C4" t="n">
-        <v>-1.8686182159355</v>
+        <v>-1.99769413663694</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0616759496058916</v>
+        <v>0.0457498302823641</v>
       </c>
       <c r="E4" t="n">
-        <v>0.166989357562271</v>
+        <v>0.160014931535711</v>
       </c>
       <c r="F4" t="n">
-        <v>1.04362816732101</v>
+        <v>0.982681773009629</v>
       </c>
       <c r="G4" t="n">
-        <v>0.41746233027044</v>
+        <v>0.396539728942166</v>
       </c>
     </row>
     <row r="5">
@@ -613,22 +613,22 @@
         <v>10</v>
       </c>
       <c r="B5" t="n">
-        <v>0.448963153953435</v>
+        <v>0.443914033175195</v>
       </c>
       <c r="C5" t="n">
-        <v>0.488043133232366</v>
+        <v>0.353812613740699</v>
       </c>
       <c r="D5" t="n">
-        <v>0.625519289385329</v>
+        <v>0.72347931979534</v>
       </c>
       <c r="E5" t="n">
-        <v>0.516418276874473</v>
+        <v>0.490174841124133</v>
       </c>
       <c r="F5" t="n">
-        <v>3.00135843094532</v>
+        <v>2.79300450971034</v>
       </c>
       <c r="G5" t="n">
-        <v>1.24497242908887</v>
+        <v>1.17006860559809</v>
       </c>
     </row>
   </sheetData>
@@ -682,28 +682,28 @@
         <v>21</v>
       </c>
       <c r="B2" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F2" t="n">
-        <v>563.733333333333</v>
+        <v>539.6875</v>
       </c>
       <c r="G2" t="n">
-        <v>91.9978969163809</v>
+        <v>89.3352498470474</v>
       </c>
       <c r="H2" t="n">
-        <v>400</v>
+        <v>399.5</v>
       </c>
       <c r="I2" t="n">
-        <v>355</v>
+        <v>336</v>
       </c>
       <c r="J2" t="n">
         <v>854</v>
@@ -746,28 +746,28 @@
         <v>23</v>
       </c>
       <c r="B4" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C4" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D4" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E4" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F4" t="n">
-        <v>292.518518518519</v>
+        <v>287.035714285714</v>
       </c>
       <c r="G4" t="n">
-        <v>27.0588126602017</v>
+        <v>26.6421142247463</v>
       </c>
       <c r="H4" t="n">
-        <v>274</v>
+        <v>273.5</v>
       </c>
       <c r="I4" t="n">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="J4" t="n">
         <v>392</v>
@@ -1312,22 +1312,22 @@
         <v>32</v>
       </c>
       <c r="B2" t="n">
-        <v>61.646351528879</v>
+        <v>61.6463515288789</v>
       </c>
       <c r="C2" t="n">
-        <v>0.131659843232311</v>
+        <v>0.131659843232312</v>
       </c>
       <c r="D2" t="n">
         <v>0.895253349399446</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0000000000000000000000000000000000000000000000001125682771932</v>
+        <v>0.000000000000000000000000000000000000000000000000112568277193212</v>
       </c>
       <c r="F2" t="s">
         <v>33</v>
       </c>
       <c r="G2" t="n">
-        <v>3348.77195875451</v>
+        <v>3348.77195875469</v>
       </c>
     </row>
     <row r="3">
@@ -1335,13 +1335,13 @@
         <v>34</v>
       </c>
       <c r="B3" t="n">
-        <v>38323732.4486327</v>
+        <v>38323732.5619672</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.00258440917112054</v>
+        <v>-0.00258440916592485</v>
       </c>
       <c r="D3" t="n">
-        <v>0.997937942119039</v>
+        <v>0.997937942123184</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -1361,19 +1361,19 @@
         <v>153.700235842784</v>
       </c>
       <c r="C4" t="n">
-        <v>0.395600299235897</v>
+        <v>0.395600299235896</v>
       </c>
       <c r="D4" t="n">
-        <v>0.692399916315753</v>
+        <v>0.692399916315754</v>
       </c>
       <c r="E4" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000377487545173725</v>
+        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000377487545173532</v>
       </c>
       <c r="F4" t="s">
         <v>37</v>
       </c>
       <c r="G4" t="n">
-        <v>255141185400050386768756736</v>
+        <v>255141185400005066273849344</v>
       </c>
     </row>
     <row r="5">
@@ -1387,16 +1387,16 @@
         <v>2.81848633729382</v>
       </c>
       <c r="D5" t="n">
-        <v>0.00482506644640399</v>
+        <v>0.00482506644640395</v>
       </c>
       <c r="E5" t="n">
-        <v>382068.8842405</v>
+        <v>382068.884240511</v>
       </c>
       <c r="F5" t="s">
         <v>39</v>
       </c>
       <c r="G5" t="n">
-        <v>2117846415518244864</v>
+        <v>2117846415518274816</v>
       </c>
     </row>
     <row r="6">
@@ -1407,19 +1407,19 @@
         <v>23.9561745009308</v>
       </c>
       <c r="C6" t="n">
-        <v>0.719541281495004</v>
+        <v>0.719541281495003</v>
       </c>
       <c r="D6" t="n">
-        <v>0.471807476334453</v>
+        <v>0.471807476334454</v>
       </c>
       <c r="E6" t="n">
-        <v>0.000000000000124336756882828</v>
+        <v>0.000000000000124336756882823</v>
       </c>
       <c r="F6" t="s">
         <v>41</v>
       </c>
       <c r="G6" t="n">
-        <v>30628959.2503676</v>
+        <v>30628959.2503669</v>
       </c>
     </row>
     <row r="7">
@@ -1427,22 +1427,22 @@
         <v>42</v>
       </c>
       <c r="B7" t="n">
-        <v>81.5462546620844</v>
+        <v>81.5462546620843</v>
       </c>
       <c r="C7" t="n">
-        <v>0.754915612260259</v>
+        <v>0.754915612260255</v>
       </c>
       <c r="D7" t="n">
-        <v>0.450299617579022</v>
+        <v>0.450299617579024</v>
       </c>
       <c r="E7" t="n">
-        <v>0.000000000000000000000000000000000000000000210428881025276</v>
+        <v>0.000000000000000000000000000000000000000000210428881025237</v>
       </c>
       <c r="F7" t="s">
         <v>43</v>
       </c>
       <c r="G7" t="n">
-        <v>543754867399032139587518464</v>
+        <v>543754867398827355546845184</v>
       </c>
     </row>
     <row r="8">
@@ -1450,22 +1450,22 @@
         <v>44</v>
       </c>
       <c r="B8" t="n">
-        <v>31.6576285786488</v>
+        <v>31.6576285786489</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.732410228391202</v>
+        <v>-0.732410228391203</v>
       </c>
       <c r="D8" t="n">
         <v>0.463918217624204</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0000000000000000000000000000000000000962198617114453</v>
+        <v>0.000000000000000000000000000000000000096219861711433</v>
       </c>
       <c r="F8" t="s">
         <v>45</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0000000000851700748783902</v>
+        <v>0.0000000000851700748783847</v>
       </c>
     </row>
     <row r="9">
@@ -1476,19 +1476,19 @@
         <v>33.8261667896644</v>
       </c>
       <c r="C9" t="n">
-        <v>0.840357807183923</v>
+        <v>0.840357807183922</v>
       </c>
       <c r="D9" t="n">
-        <v>0.40070779861187</v>
+        <v>0.400707798611871</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0000000000000000356784326903035</v>
+        <v>0.000000000000000035678432690302</v>
       </c>
       <c r="F9" t="s">
         <v>47</v>
       </c>
       <c r="G9" t="n">
-        <v>2214578812114.3</v>
+        <v>2214578812114.25</v>
       </c>
     </row>
     <row r="10">
@@ -1499,19 +1499,19 @@
         <v>167.242428728349</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.804903503961642</v>
+        <v>-0.80490350396164</v>
       </c>
       <c r="D10" t="n">
-        <v>0.420875366242144</v>
+        <v>0.420875366242145</v>
       </c>
       <c r="E10" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000151656787184261</v>
+        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000151656787184304</v>
       </c>
       <c r="F10" t="s">
         <v>49</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000345044632466977</v>
+        <v>0.0000000000000000000000000000000000000000000000000000000000345044632467085</v>
       </c>
     </row>
     <row r="11">
@@ -1522,19 +1522,19 @@
         <v>207.962366767297</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.424828918122422</v>
+        <v>-0.424828918122417</v>
       </c>
       <c r="D11" t="n">
-        <v>0.670961395180726</v>
+        <v>0.67096139518073</v>
       </c>
       <c r="E11" t="n">
-        <v>4.10088908077937e-216</v>
+        <v>4.1008890807866e-216</v>
       </c>
       <c r="F11" t="s">
         <v>51</v>
       </c>
       <c r="G11" t="n">
-        <v>0.00000000000000000000000000000000000000427332128261039</v>
+        <v>0.00000000000000000000000000000000000000427332128261592</v>
       </c>
     </row>
     <row r="12">
@@ -1548,10 +1548,10 @@
         <v>-2.63634092891602</v>
       </c>
       <c r="D12" t="n">
-        <v>0.00838054830599798</v>
+        <v>0.00838054830599803</v>
       </c>
       <c r="E12" t="n">
-        <v>0.00000753460070200555</v>
+        <v>0.00000753460070200553</v>
       </c>
       <c r="F12" t="s">
         <v>53</v>
@@ -1565,16 +1565,16 @@
         <v>28</v>
       </c>
       <c r="B13" t="n">
-        <v>1.08929723803791</v>
+        <v>1.0892972380379</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.308669847036519</v>
+        <v>-0.30866984703652</v>
       </c>
       <c r="D13" t="n">
-        <v>0.757572683059894</v>
+        <v>0.757572683059893</v>
       </c>
       <c r="E13" t="n">
-        <v>0.084482018434504</v>
+        <v>0.084482018434505</v>
       </c>
       <c r="F13" t="s">
         <v>54</v>
@@ -1588,16 +1588,16 @@
         <v>29</v>
       </c>
       <c r="B14" t="n">
-        <v>1.06674239484188</v>
+        <v>1.06674239484187</v>
       </c>
       <c r="C14" t="n">
-        <v>1.09337612997911</v>
+        <v>1.09337612997912</v>
       </c>
       <c r="D14" t="n">
-        <v>0.274228689512069</v>
+        <v>0.274228689512066</v>
       </c>
       <c r="E14" t="n">
-        <v>0.396759092130491</v>
+        <v>0.396759092130496</v>
       </c>
       <c r="F14" t="s">
         <v>55</v>

</xml_diff>